<commit_message>
Raghav Bansal Changes 29.10.2019
</commit_message>
<xml_diff>
--- a/Databases/BackendTables.xlsx
+++ b/Databases/BackendTables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CCAS\Databases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E57828B-7E49-4125-BE36-2E1C9E4B349E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8452E142-2CB9-438B-A60D-A3FF917BE943}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1A15F2D6-129E-42C9-9251-2D56C0680DA1}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="67">
   <si>
     <t>Login_Details</t>
   </si>
@@ -218,9 +218,6 @@
     <t>COE_times</t>
   </si>
   <si>
-    <t xml:space="preserve">Event_Sponsors </t>
-  </si>
-  <si>
     <t>E20190001</t>
   </si>
   <si>
@@ -228,6 +225,12 @@
   </si>
   <si>
     <t>Workshop_Details NOT FINAL</t>
+  </si>
+  <si>
+    <t>Event_Sponsor</t>
+  </si>
+  <si>
+    <t>Society_Name</t>
   </si>
 </sst>
 </file>
@@ -251,7 +254,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -276,6 +279,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -289,7 +298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -303,6 +312,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -617,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B2E7121-147F-491D-A668-533D9D4655A8}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -682,7 +692,7 @@
         <v>41</v>
       </c>
       <c r="J3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -701,7 +711,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
@@ -728,189 +738,200 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" t="s">
-        <v>58</v>
-      </c>
+      <c r="A7" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" t="s">
-        <v>46</v>
+        <v>2</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="H8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="F9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
+        <v>4</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="F10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>65</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F11" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="H11" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="F14" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>9</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C16" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
         <v>30</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F17" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" t="s">
         <v>31</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F18" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="F19" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>6</v>
+        <v>14</v>
+      </c>
+      <c r="C24" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>15</v>
+      </c>
+      <c r="C25" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>